<commit_message>
some modifications for solving a jmol bug in DB visualisation: now using pubchem as source of vis
</commit_message>
<xml_diff>
--- a/Fitting-Values.xlsx
+++ b/Fitting-Values.xlsx
@@ -5,19 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="florent_krystel_values" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="florent_difflc_nma" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="florent_krystel_dg" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="florent_nma_new" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="krystel_dh_rho" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="tab 12" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="230">
   <si>
     <t>Parameters from Krsystel using original scripts from Tristan with or without interface</t>
   </si>
@@ -454,12 +457,18 @@
     <t>Benzonitrile (MTP 2)</t>
   </si>
   <si>
+    <t>CIS NMA</t>
+  </si>
+  <si>
     <t>NMA (unscaled, Tristan article)</t>
   </si>
   <si>
     <t>NMA (unscaled, interface)</t>
   </si>
   <si>
+    <t>CGENFF last</t>
+  </si>
+  <si>
     <t>NMA (scaled 1.025, interface)</t>
   </si>
   <si>
@@ -479,6 +488,228 @@
   </si>
   <si>
     <t>NMA (unscaled, lambda breaking 3)</t>
+  </si>
+  <si>
+    <t>TRANS NMA</t>
+  </si>
+  <si>
+    <t>DRUDE</t>
+  </si>
+  <si>
+    <t>NMA  CIS</t>
+  </si>
+  <si>
+    <t>CGENFF DRUDE</t>
+  </si>
+  <si>
+    <t>NMA  TRANS</t>
+  </si>
+  <si>
+    <t>NEW RESULTS</t>
+  </si>
+  <si>
+    <t>TRANS</t>
+  </si>
+  <si>
+    <t>CIS</t>
+  </si>
+  <si>
+    <t>NMA TRANS NMA (unscaled, interface)</t>
+  </si>
+  <si>
+    <t>NO MTP (PC ONLY) breaking auto</t>
+  </si>
+  <si>
+    <t>Fitted -OH</t>
+  </si>
+  <si>
+    <t>Phenol </t>
+  </si>
+  <si>
+    <t>Exp.</t>
+  </si>
+  <si>
+    <t>Gas-mtp</t>
+  </si>
+  <si>
+    <t>Gas-vdw</t>
+  </si>
+  <si>
+    <t>Solvent-mtp</t>
+  </si>
+  <si>
+    <t>Solvent-vdw</t>
+  </si>
+  <si>
+    <t>This is for a density correlation plot.</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>EXP / Predicted</t>
+  </si>
+  <si>
+    <t>MTP / calc</t>
+  </si>
+  <si>
+    <t>deviation</t>
+  </si>
+  <si>
+    <t>Bromo-phenol-pyridine</t>
+  </si>
+  <si>
+    <t>Bromo-aniline-pyridine</t>
+  </si>
+  <si>
+    <t>Bromopyridine-nhch3</t>
+  </si>
+  <si>
+    <t>6-chloropyridin-3-ol</t>
+  </si>
+  <si>
+    <t>6-chloropyridin-3-amine</t>
+  </si>
+  <si>
+    <t>6-chlo-N-methylpyridin-3-amine</t>
+  </si>
+  <si>
+    <t>p-chlorophenol</t>
+  </si>
+  <si>
+    <t>p-chloroaniline</t>
+  </si>
+  <si>
+    <t>N-Methyl-(p-chlorophenyl)amine</t>
+  </si>
+  <si>
+    <t>4-bromo-N-methylaniline</t>
+  </si>
+  <si>
+    <t>4-bromoaniline</t>
+  </si>
+  <si>
+    <t>4-bromophenol</t>
+  </si>
+  <si>
+    <t>2-fluoropyridine</t>
+  </si>
+  <si>
+    <t>2-chloropyridine</t>
+  </si>
+  <si>
+    <t>2-bromopyridine</t>
+  </si>
+  <si>
+    <t>4-fluorophenol</t>
+  </si>
+  <si>
+    <t>4-fluoroaniline</t>
+  </si>
+  <si>
+    <t>4-fluoro-N-methylaniline</t>
+  </si>
+  <si>
+    <t>New values (including fitted vdw for the new fragments)</t>
+  </si>
+  <si>
+    <t>delta H</t>
+  </si>
+  <si>
+    <t>My contribution to Table 12</t>
+  </si>
+  <si>
+    <t>Chlorophenol</t>
+  </si>
+  <si>
+    <t>heat of vap</t>
+  </si>
+  <si>
+    <t>solvation</t>
+  </si>
+  <si>
+    <t>CGenFF (PC and LJ)</t>
+  </si>
+  <si>
+    <t>opt PC / CGenFF LJ</t>
+  </si>
+  <si>
+    <t>opt PC / opt LJ</t>
+  </si>
+  <si>
+    <t>opt MTP / CGenFF LJ</t>
+  </si>
+  <si>
+    <t>opt MTP / opt LJ</t>
+  </si>
+  <si>
+    <t>                     </t>
+  </si>
+  <si>
+    <t> $\rho$ </t>
+  </si>
+  <si>
+    <t> $\Delta H_{vap}$ (kcal/mol) </t>
+  </si>
+  <si>
+    <t> $\Delta G_{hyd}$ (kcal/mol) \\ \hline</t>
+  </si>
+  <si>
+    <t>NMA        </t>
+  </si>
+  <si>
+    <t> Exp.     </t>
+  </si>
+  <si>
+    <t>           -10.10            \\</t>
+  </si>
+  <si>
+    <t> CGenFF (PC and LJ)  </t>
+  </si>
+  <si>
+    <t>           -11.03            \\</t>
+  </si>
+  <si>
+    <t> opt PC / CGenFF LJ  </t>
+  </si>
+  <si>
+    <t>           -10.11            \\</t>
+  </si>
+  <si>
+    <t> opt PC / opt LJ     </t>
+  </si>
+  <si>
+    <t> opt MTP / CGenFF LJ </t>
+  </si>
+  <si>
+    <t>            -9.88            \\</t>
+  </si>
+  <si>
+    <t> opt MTP / opt LJ    </t>
+  </si>
+  <si>
+    <t>            -8.07            \\</t>
+  </si>
+  <si>
+    <t>4-ClPhenol </t>
+  </si>
+  <si>
+    <t>            -7.03            \\</t>
+  </si>
+  <si>
+    <t>            -5.47            \\</t>
+  </si>
+  <si>
+    <t>            -5.44            \\</t>
+  </si>
+  <si>
+    <t>            -5.61            \\</t>
+  </si>
+  <si>
+    <t>            -5.91            \\</t>
+  </si>
+  <si>
+    <t>            -7.14            \\ \hline</t>
   </si>
 </sst>
 </file>
@@ -489,7 +720,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -620,6 +851,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF009900"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -677,7 +916,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -880,6 +1119,42 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -942,7 +1217,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF009900"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -959,15 +1234,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>222480</xdr:colOff>
+      <xdr:colOff>303480</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>142920</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19440</xdr:colOff>
+      <xdr:colOff>99360</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -980,8 +1255,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1751400" y="20703240"/>
-          <a:ext cx="5485320" cy="3492000"/>
+          <a:off x="1832400" y="20676240"/>
+          <a:ext cx="5484240" cy="3490920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -996,15 +1271,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>232200</xdr:colOff>
+      <xdr:colOff>313200</xdr:colOff>
       <xdr:row>147</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>101520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>29160</xdr:colOff>
-      <xdr:row>169</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:colOff>109080</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1017,8 +1292,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1761120" y="24431760"/>
-          <a:ext cx="5485320" cy="3492000"/>
+          <a:off x="1842120" y="24404760"/>
+          <a:ext cx="5484240" cy="3490920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1033,15 +1308,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>211320</xdr:colOff>
+      <xdr:colOff>292320</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>115560</xdr:rowOff>
+      <xdr:rowOff>88560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
+      <xdr:colOff>88200</xdr:colOff>
       <xdr:row>192</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1054,8 +1329,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1740240" y="28186200"/>
-          <a:ext cx="5485320" cy="3492000"/>
+          <a:off x="1821240" y="28159200"/>
+          <a:ext cx="5484240" cy="3490920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1070,15 +1345,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>208080</xdr:colOff>
+      <xdr:colOff>289080</xdr:colOff>
       <xdr:row>193</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>5040</xdr:colOff>
-      <xdr:row>215</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:colOff>84960</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1091,8 +1366,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1737000" y="31896000"/>
-          <a:ext cx="5485320" cy="3492000"/>
+          <a:off x="1818000" y="31869000"/>
+          <a:ext cx="5484240" cy="3490920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1114,8 +1389,8 @@
   </sheetPr>
   <dimension ref="A3:O164"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C105" activeCellId="0" sqref="C105"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2494,11 +2769,11 @@
         <v>1</v>
       </c>
       <c r="B86" s="21" t="n">
-        <f aca="false">D57</f>
+        <f aca="false">florent_krystel_values!D57</f>
         <v>0.95</v>
       </c>
       <c r="C86" s="21" t="n">
-        <f aca="false">D58</f>
+        <f aca="false">florent_krystel_values!D58</f>
         <v>13.82</v>
       </c>
       <c r="D86" s="22" t="n">
@@ -2519,11 +2794,11 @@
         <v>1.025</v>
       </c>
       <c r="B87" s="21" t="n">
-        <f aca="false">C77</f>
+        <f aca="false">florent_krystel_values!C77</f>
         <v>0.915</v>
       </c>
       <c r="C87" s="21" t="n">
-        <f aca="false">C78</f>
+        <f aca="false">florent_krystel_values!C78</f>
         <v>13.68</v>
       </c>
       <c r="D87" s="33" t="n">
@@ -2538,11 +2813,11 @@
         <v>1.05</v>
       </c>
       <c r="B88" s="21" t="n">
-        <f aca="false">C67</f>
+        <f aca="false">florent_krystel_values!C67</f>
         <v>0.883</v>
       </c>
       <c r="C88" s="21" t="n">
-        <f aca="false">C68</f>
+        <f aca="false">florent_krystel_values!C68</f>
         <v>13.569</v>
       </c>
       <c r="D88" s="33" t="n">
@@ -2569,11 +2844,11 @@
         <v>1.075</v>
       </c>
       <c r="B89" s="21" t="n">
-        <f aca="false">D77</f>
+        <f aca="false">florent_krystel_values!D77</f>
         <v>0.843</v>
       </c>
       <c r="C89" s="21" t="n">
-        <f aca="false">D78</f>
+        <f aca="false">florent_krystel_values!D78</f>
         <v>13.29</v>
       </c>
       <c r="D89" s="33" t="n">
@@ -2600,11 +2875,11 @@
         <v>1.1</v>
       </c>
       <c r="B90" s="21" t="n">
-        <f aca="false">D67</f>
+        <f aca="false">florent_krystel_values!D67</f>
         <v>0.805</v>
       </c>
       <c r="C90" s="21" t="n">
-        <f aca="false">D68</f>
+        <f aca="false">florent_krystel_values!D68</f>
         <v>13.469</v>
       </c>
       <c r="D90" s="33" t="n">
@@ -2875,7 +3150,7 @@
   </sheetPr>
   <dimension ref="B2:W22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -3376,24 +3651,91 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="G7:P38"/>
+  <dimension ref="G1:P62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q85" activeCellId="0" sqref="Q85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="9" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="9" width="42.469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="9" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="18.8469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="24.6122448979592"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="9" width="17.3061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="9" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="9" width="52.2755102040816"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="9" width="33.6938775510204"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="9" width="11.5204081632653"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0"/>
+      <c r="P6" s="0"/>
+    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G7" s="9" t="s">
         <v>125</v>
@@ -3404,6 +3746,12 @@
       <c r="I7" s="9" t="s">
         <v>127</v>
       </c>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="9" t="s">
@@ -3415,6 +3763,12 @@
       <c r="I8" s="9" t="n">
         <v>-0.86</v>
       </c>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="9" t="s">
@@ -3426,6 +3780,12 @@
       <c r="I9" s="9" t="n">
         <v>-0.34</v>
       </c>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="9" t="s">
@@ -3437,6 +3797,12 @@
       <c r="I10" s="16" t="n">
         <v>-6.49713999999999</v>
       </c>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="0"/>
+      <c r="O10" s="0"/>
+      <c r="P10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="9" t="s">
@@ -3448,7 +3814,12 @@
       <c r="I11" s="9" t="n">
         <v>-0.89</v>
       </c>
+      <c r="J11" s="0"/>
       <c r="K11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G12" s="9" t="s">
@@ -3460,7 +3831,12 @@
       <c r="I12" s="9" t="n">
         <v>-0.75</v>
       </c>
+      <c r="J12" s="0"/>
       <c r="K12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G13" s="9" t="s">
@@ -3472,7 +3848,12 @@
       <c r="I13" s="16" t="n">
         <v>-1.11</v>
       </c>
+      <c r="J13" s="0"/>
       <c r="K13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G14" s="9" t="s">
@@ -3484,7 +3865,12 @@
       <c r="I14" s="9" t="n">
         <v>-1.4</v>
       </c>
+      <c r="J14" s="0"/>
       <c r="K14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
+      <c r="O14" s="0"/>
+      <c r="P14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G15" s="9" t="s">
@@ -3496,7 +3882,12 @@
       <c r="I15" s="9" t="n">
         <v>-1.97</v>
       </c>
+      <c r="J15" s="0"/>
       <c r="K15" s="0"/>
+      <c r="M15" s="0"/>
+      <c r="N15" s="0"/>
+      <c r="O15" s="0"/>
+      <c r="P15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G16" s="9" t="s">
@@ -3508,7 +3899,12 @@
       <c r="I16" s="9" t="n">
         <v>-3.74</v>
       </c>
+      <c r="J16" s="0"/>
       <c r="K16" s="0"/>
+      <c r="M16" s="0"/>
+      <c r="N16" s="0"/>
+      <c r="O16" s="0"/>
+      <c r="P16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G17" s="9" t="s">
@@ -3520,6 +3916,11 @@
       <c r="I17" s="9" t="n">
         <v>-0.77</v>
       </c>
+      <c r="J17" s="0"/>
+      <c r="M17" s="0"/>
+      <c r="N17" s="0"/>
+      <c r="O17" s="0"/>
+      <c r="P17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G18" s="9" t="s">
@@ -3531,6 +3932,11 @@
       <c r="I18" s="9" t="n">
         <v>-0.48</v>
       </c>
+      <c r="J18" s="0"/>
+      <c r="M18" s="0"/>
+      <c r="N18" s="0"/>
+      <c r="O18" s="0"/>
+      <c r="P18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G19" s="9" t="s">
@@ -3542,6 +3948,11 @@
       <c r="I19" s="16" t="n">
         <v>-0.66</v>
       </c>
+      <c r="J19" s="0"/>
+      <c r="M19" s="0"/>
+      <c r="N19" s="0"/>
+      <c r="O19" s="0"/>
+      <c r="P19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G20" s="9" t="s">
@@ -3553,6 +3964,8 @@
       <c r="I20" s="9" t="n">
         <v>-0.55</v>
       </c>
+      <c r="J20" s="0"/>
+      <c r="M20" s="0"/>
       <c r="N20" s="45"/>
       <c r="O20" s="46"/>
       <c r="P20" s="47"/>
@@ -3567,6 +3980,8 @@
       <c r="I21" s="9" t="n">
         <v>-1.35</v>
       </c>
+      <c r="J21" s="0"/>
+      <c r="M21" s="0"/>
       <c r="N21" s="45"/>
       <c r="O21" s="46"/>
       <c r="P21" s="47"/>
@@ -3581,6 +3996,8 @@
       <c r="I22" s="9" t="n">
         <v>-4.11</v>
       </c>
+      <c r="J22" s="0"/>
+      <c r="M22" s="0"/>
       <c r="N22" s="45"/>
       <c r="O22" s="46"/>
       <c r="P22" s="47"/>
@@ -3595,6 +4012,8 @@
       <c r="I23" s="48" t="n">
         <v>-6.496</v>
       </c>
+      <c r="J23" s="0"/>
+      <c r="M23" s="0"/>
       <c r="N23" s="45"/>
       <c r="O23" s="46"/>
       <c r="P23" s="47"/>
@@ -3610,6 +4029,9 @@
         <f aca="false">(-19.9386+15.02058)-(-13.1343+11.98497)</f>
         <v>-3.76869</v>
       </c>
+      <c r="J24" s="0"/>
+      <c r="M24" s="0"/>
+      <c r="N24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G25" s="9" t="s">
@@ -3622,6 +4044,9 @@
         <f aca="false">(-19.81878+15.4574)-(-13.12671+12.50767)</f>
         <v>-3.74234</v>
       </c>
+      <c r="J25" s="0"/>
+      <c r="M25" s="0"/>
+      <c r="N25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G26" s="9" t="s">
@@ -3633,6 +4058,9 @@
       <c r="I26" s="49" t="n">
         <v>-3.9</v>
       </c>
+      <c r="J26" s="0"/>
+      <c r="M26" s="0"/>
+      <c r="N26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G27" s="9" t="s">
@@ -3644,17 +4072,15 @@
       <c r="I27" s="49" t="n">
         <v>-4.74</v>
       </c>
+      <c r="J27" s="0"/>
+      <c r="M27" s="0"/>
+      <c r="N27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G28" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H28" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I28" s="50" t="n">
-        <v>-7.34</v>
-      </c>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="I28" s="0"/>
+      <c r="J28" s="0"/>
       <c r="M28" s="42" t="s">
         <v>87</v>
       </c>
@@ -3663,58 +4089,38 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G29" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H29" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I29" s="50" t="n">
-        <v>-7.09</v>
-      </c>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
       <c r="M29" s="0"/>
       <c r="N29" s="42" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G30" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H30" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I30" s="48" t="n">
-        <v>-6.37</v>
-      </c>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
       <c r="M30" s="0"/>
       <c r="N30" s="42" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G31" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H31" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I31" s="48" t="n">
-        <v>-6.21</v>
-      </c>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
       <c r="M31" s="0"/>
       <c r="N31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G32" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="H32" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I32" s="48" t="n">
-        <v>-5.68</v>
-      </c>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
       <c r="M32" s="42" t="s">
         <v>91</v>
       </c>
@@ -3723,58 +4129,38 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G33" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I33" s="48" t="n">
-        <v>-5.67</v>
-      </c>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="0"/>
       <c r="M33" s="0"/>
       <c r="N33" s="42" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G34" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H34" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I34" s="49" t="n">
-        <v>-3.81</v>
-      </c>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
       <c r="M34" s="0"/>
       <c r="N34" s="42" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G35" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="H35" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I35" s="49" t="n">
-        <v>-6.22</v>
-      </c>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
       <c r="M35" s="0"/>
       <c r="N35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G36" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="H36" s="50" t="n">
-        <v>-10</v>
-      </c>
-      <c r="I36" s="49" t="n">
-        <v>-6.89</v>
-      </c>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
+      <c r="J36" s="0"/>
       <c r="M36" s="42" t="s">
         <v>94</v>
       </c>
@@ -3783,15 +4169,243 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
+      <c r="I37" s="0"/>
+      <c r="J37" s="0"/>
       <c r="M37" s="0"/>
       <c r="N37" s="42" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
+      <c r="J38" s="0"/>
       <c r="M38" s="0"/>
       <c r="N38" s="42" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="J39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
+      <c r="I40" s="0"/>
+      <c r="J40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
+      <c r="J41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
+      <c r="I42" s="0"/>
+      <c r="J42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
+      <c r="I43" s="0"/>
+      <c r="J43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G44" s="0"/>
+      <c r="H44" s="0"/>
+      <c r="I44" s="0"/>
+      <c r="J44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G45" s="0"/>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="J45" s="0"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="J46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G47" s="0"/>
+      <c r="H47" s="0"/>
+      <c r="I47" s="0"/>
+      <c r="J47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G48" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G49" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H49" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I49" s="50" t="n">
+        <v>-7.34</v>
+      </c>
+      <c r="J49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G50" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H50" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I50" s="50" t="n">
+        <v>-7.09</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H51" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I51" s="48" t="n">
+        <v>-6.37</v>
+      </c>
+      <c r="J51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H52" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I52" s="48" t="n">
+        <v>-6.21</v>
+      </c>
+      <c r="J52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G53" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H53" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I53" s="48" t="n">
+        <v>-5.68</v>
+      </c>
+      <c r="J53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G54" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H54" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I54" s="48" t="n">
+        <v>-5.67</v>
+      </c>
+      <c r="J54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G55" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H55" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I55" s="49" t="n">
+        <v>-3.81</v>
+      </c>
+      <c r="J55" s="0"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G56" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H56" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I56" s="49" t="n">
+        <v>-6.22</v>
+      </c>
+      <c r="J56" s="0"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G57" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H57" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="I57" s="49" t="n">
+        <v>-6.89</v>
+      </c>
+      <c r="J57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G58" s="0"/>
+      <c r="H58" s="0"/>
+      <c r="I58" s="0"/>
+      <c r="J58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G59" s="0"/>
+      <c r="H59" s="0"/>
+      <c r="I59" s="0"/>
+      <c r="J59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G60" s="0"/>
+      <c r="H60" s="0"/>
+      <c r="I60" s="0"/>
+      <c r="J60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G61" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J61" s="0"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G62" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H62" s="9" t="n">
+        <v>-9.8</v>
+      </c>
+      <c r="I62" s="9" t="n">
+        <v>-8.67</v>
+      </c>
+      <c r="J62" s="9" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3803,4 +4417,1352 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C3" s="50" t="n">
+        <v>-7.34</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C4" s="50" t="n">
+        <v>-7.09</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C5" s="48" t="n">
+        <v>-6.37</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C6" s="48" t="n">
+        <v>-6.21</v>
+      </c>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C7" s="48" t="n">
+        <v>-5.68</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C8" s="48" t="n">
+        <v>-5.67</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C9" s="49" t="n">
+        <v>-3.81</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C10" s="49" t="n">
+        <v>-6.22</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="50" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="C11" s="49" t="n">
+        <v>-6.89</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="9" t="n">
+        <v>-10.1</v>
+      </c>
+      <c r="C16" s="9" t="n">
+        <v>-8.67</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="43" t="n">
+        <v>-9.81</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" s="9" t="n">
+        <v>-10.1</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>-9.88</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="9" t="n">
+        <v>-10.1</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>-8.06</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="9" t="n">
+        <v>-10.1</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>-11.02</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A3:D78"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E76" activeCellId="0" sqref="E76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="52" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>-13.10672</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>11.43361</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>-21.46573</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>13.31888</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11" t="n">
+        <f aca="false">B7+B8-B5-B6</f>
+        <v>-6.47374</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>-6.6</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="54" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="C17" s="54" t="n">
+        <v>1.807</v>
+      </c>
+      <c r="D17" s="55" t="n">
+        <f aca="false">C17-B17</f>
+        <v>0.0169999999999999</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="54" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="C18" s="54" t="n">
+        <v>1.6829</v>
+      </c>
+      <c r="D18" s="55" t="n">
+        <f aca="false">C18-B18</f>
+        <v>-0.0270999999999999</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" s="54" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="C19" s="54" t="n">
+        <v>1.5711</v>
+      </c>
+      <c r="D19" s="55" t="n">
+        <f aca="false">C19-B19</f>
+        <v>-0.00890000000000013</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="55"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="54" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="C21" s="54" t="n">
+        <v>1.3561</v>
+      </c>
+      <c r="D21" s="55" t="n">
+        <f aca="false">C21-B21</f>
+        <v>-0.0339</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="54" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="C22" s="54" t="n">
+        <v>1.2928</v>
+      </c>
+      <c r="D22" s="55" t="n">
+        <f aca="false">C22-B22</f>
+        <v>-0.0372000000000001</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" s="54" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="C23" s="54" t="n">
+        <v>1.211</v>
+      </c>
+      <c r="D23" s="55" t="n">
+        <f aca="false">C23-B23</f>
+        <v>-0.0389999999999999</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" s="54" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="C25" s="54" t="n">
+        <v>1.2514</v>
+      </c>
+      <c r="D25" s="55" t="n">
+        <f aca="false">C25-B25</f>
+        <v>0.0314000000000001</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="54" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="C26" s="54" t="n">
+        <v>1.1922</v>
+      </c>
+      <c r="D26" s="55" t="n">
+        <f aca="false">C26-B26</f>
+        <v>0.0222</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="54" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C27" s="54" t="n">
+        <v>1.1984</v>
+      </c>
+      <c r="D27" s="55" t="n">
+        <f aca="false">C27-B27</f>
+        <v>-0.00160000000000005</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="55"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="54" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="C29" s="54" t="n">
+        <v>1.6351</v>
+      </c>
+      <c r="D29" s="55" t="n">
+        <f aca="false">C29-B29</f>
+        <v>-0.0249000000000001</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="54" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="C30" s="54" t="n">
+        <v>1.5543</v>
+      </c>
+      <c r="D30" s="55" t="n">
+        <f aca="false">C30-B30</f>
+        <v>-0.0356999999999998</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31" s="54" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="C31" s="54" t="n">
+        <v>1.8268</v>
+      </c>
+      <c r="D31" s="55" t="n">
+        <f aca="false">C31-B31</f>
+        <v>-0.0131999999999999</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="54" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="C33" s="54" t="n">
+        <v>1.1654</v>
+      </c>
+      <c r="D33" s="55" t="n">
+        <f aca="false">C33-B33</f>
+        <v>0.0373999999999999</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="54" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C34" s="54" t="n">
+        <v>1.2113</v>
+      </c>
+      <c r="D34" s="55" t="n">
+        <f aca="false">C34-B34</f>
+        <v>0.0113000000000001</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B35" s="54" t="n">
+        <v>1.657</v>
+      </c>
+      <c r="C35" s="54" t="n">
+        <v>1.641</v>
+      </c>
+      <c r="D35" s="55" t="n">
+        <f aca="false">C35-B35</f>
+        <v>-0.016</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="55"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="54" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="C37" s="54" t="n">
+        <v>1.3163</v>
+      </c>
+      <c r="D37" s="55" t="n">
+        <f aca="false">C37-B37</f>
+        <v>0.00629999999999997</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B38" s="54" t="n">
+        <v>1.173</v>
+      </c>
+      <c r="C38" s="54" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="D38" s="55" t="n">
+        <f aca="false">C38-B38</f>
+        <v>0.0069999999999999</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B39" s="54" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="C39" s="54" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="D39" s="55" t="n">
+        <f aca="false">C39-B39</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="8"/>
+      <c r="D44" s="55"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" s="10" t="n">
+        <v>13.05</v>
+      </c>
+      <c r="C45" s="8" t="n">
+        <v>13.7218</v>
+      </c>
+      <c r="D45" s="55" t="n">
+        <f aca="false">C45-B45</f>
+        <v>0.671799999999999</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="10" t="n">
+        <v>12.67</v>
+      </c>
+      <c r="C46" s="8" t="n">
+        <v>12.1295</v>
+      </c>
+      <c r="D46" s="55" t="n">
+        <f aca="false">C46-B46</f>
+        <v>-0.5405</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" s="10" t="n">
+        <v>12.17</v>
+      </c>
+      <c r="C47" s="8" t="n">
+        <v>11.595</v>
+      </c>
+      <c r="D47" s="55" t="n">
+        <f aca="false">C47-B47</f>
+        <v>-0.574999999999999</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="55"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" s="10" t="n">
+        <v>14.81</v>
+      </c>
+      <c r="C49" s="10" t="n">
+        <v>15.3594</v>
+      </c>
+      <c r="D49" s="55" t="n">
+        <f aca="false">C49-B49</f>
+        <v>0.5494</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="10" t="n">
+        <v>12.71</v>
+      </c>
+      <c r="C50" s="8" t="n">
+        <v>12.4393</v>
+      </c>
+      <c r="D50" s="55" t="n">
+        <f aca="false">C50-B50</f>
+        <v>-0.270700000000001</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B51" s="10" t="n">
+        <v>12.28</v>
+      </c>
+      <c r="C51" s="8" t="n">
+        <v>11.5954</v>
+      </c>
+      <c r="D51" s="55" t="n">
+        <f aca="false">C51-B51</f>
+        <v>-0.6846</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="55"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="10" t="n">
+        <v>11.243</v>
+      </c>
+      <c r="C53" s="10" t="n">
+        <v>10.4589</v>
+      </c>
+      <c r="D53" s="55" t="n">
+        <f aca="false">C53-B53</f>
+        <v>-0.7841</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B54" s="10" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="C54" s="8" t="n">
+        <v>10.5074</v>
+      </c>
+      <c r="D54" s="55" t="n">
+        <f aca="false">C54-B54</f>
+        <v>-0.692599999999999</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B55" s="10" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="C55" s="56" t="n">
+        <v>12.0824</v>
+      </c>
+      <c r="D55" s="55" t="n">
+        <f aca="false">C55-B55</f>
+        <v>0.682399999999999</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="55"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B57" s="10" t="n">
+        <v>11.22</v>
+      </c>
+      <c r="C57" s="8" t="n">
+        <v>11.4997</v>
+      </c>
+      <c r="D57" s="55" t="n">
+        <f aca="false">C57-B57</f>
+        <v>0.2797</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58" s="10" t="n">
+        <v>11.74</v>
+      </c>
+      <c r="C58" s="10" t="n">
+        <v>12.3756</v>
+      </c>
+      <c r="D58" s="55" t="n">
+        <f aca="false">C58-B58</f>
+        <v>0.6356</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" s="10" t="n">
+        <v>14.04</v>
+      </c>
+      <c r="C59" s="8" t="n">
+        <v>14.1048</v>
+      </c>
+      <c r="D59" s="55" t="n">
+        <f aca="false">C59-B59</f>
+        <v>0.0648000000000017</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="55"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61" s="10" t="n">
+        <v>8.215</v>
+      </c>
+      <c r="C61" s="10" t="n">
+        <v>8.674</v>
+      </c>
+      <c r="D61" s="55" t="n">
+        <f aca="false">C61-B61</f>
+        <v>0.459</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B62" s="10" t="n">
+        <v>10.18</v>
+      </c>
+      <c r="C62" s="10" t="n">
+        <v>9.926</v>
+      </c>
+      <c r="D62" s="55" t="n">
+        <f aca="false">C62-B62</f>
+        <v>-0.254</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B63" s="10" t="n">
+        <v>9.947</v>
+      </c>
+      <c r="C63" s="8" t="n">
+        <v>9.5312</v>
+      </c>
+      <c r="D63" s="55" t="n">
+        <f aca="false">C63-B63</f>
+        <v>-0.415799999999999</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="55"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B65" s="10" t="n">
+        <v>10.43</v>
+      </c>
+      <c r="C65" s="10" t="n">
+        <v>10.7679</v>
+      </c>
+      <c r="D65" s="55" t="n">
+        <f aca="false">C65-B65</f>
+        <v>0.337900000000001</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" s="10" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="C66" s="10" t="n">
+        <v>9.4311</v>
+      </c>
+      <c r="D66" s="55" t="n">
+        <f aca="false">C66-B66</f>
+        <v>-0.728899999999999</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B67" s="10" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="C67" s="8" t="n">
+        <v>10.0646</v>
+      </c>
+      <c r="D67" s="55" t="n">
+        <f aca="false">C67-B67</f>
+        <v>0.0846</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="52" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="8" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="C73" s="8" t="n">
+        <v>11.24</v>
+      </c>
+      <c r="D73" s="8" t="n">
+        <v>-7.03</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="B74" s="10" t="n">
+        <v>1.2759</v>
+      </c>
+      <c r="C74" s="10" t="n">
+        <v>15.7423</v>
+      </c>
+      <c r="D74" s="10" t="n">
+        <v>-5.46989</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="B75" s="10" t="n">
+        <v>1.2737</v>
+      </c>
+      <c r="C75" s="10" t="n">
+        <v>10.7761</v>
+      </c>
+      <c r="D75" s="10" t="n">
+        <v>-5.43556</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" s="10" t="n">
+        <v>1.2471</v>
+      </c>
+      <c r="C76" s="10" t="n">
+        <v>11.849</v>
+      </c>
+      <c r="D76" s="10" t="n">
+        <v>-5.60644</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="B77" s="10" t="n">
+        <v>1.2684</v>
+      </c>
+      <c r="C77" s="10" t="n">
+        <v>12.858</v>
+      </c>
+      <c r="D77" s="10" t="n">
+        <v>-5.91251</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="B78" s="10" t="n">
+        <v>1.2514</v>
+      </c>
+      <c r="C78" s="10" t="n">
+        <v>11.4589</v>
+      </c>
+      <c r="D78" s="59" t="n">
+        <v>-7.14277</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="D13:H25"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.5051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>15.09</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>14.49</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>13.47</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>11.24</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>15.74</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>11.85</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>12.86</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>11.46</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>